<commit_message>
correct answers now supported
</commit_message>
<xml_diff>
--- a/services/tps/inputs/TEMPLATE_DISTRATOR.xlsx
+++ b/services/tps/inputs/TEMPLATE_DISTRATOR.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22702"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x05898109102\Documents\ppa\services\destrator\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-audrs\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC7A9286-AFB8-4F45-9A45-BC25CE17899B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PERFORMANCE" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
     <definedName name="Title2">#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">PERFORMANCE!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -59,6 +60,9 @@
     <t>RELATÓRIO DE PERFORMANCE</t>
   </si>
   <si>
+    <t>DISTRATORES</t>
+  </si>
+  <si>
     <t>MAIOR: 10</t>
   </si>
   <si>
@@ -71,7 +75,7 @@
     <t>DESVIO: 0</t>
   </si>
   <si>
-    <t>Matriz de Destratores</t>
+    <t>Matriz de Distratores</t>
   </si>
   <si>
     <t xml:space="preserve">      </t>
@@ -120,15 +124,12 @@
   </si>
   <si>
     <t xml:space="preserve">      Q. 10</t>
-  </si>
-  <si>
-    <t>DISTRATORES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -136,7 +137,7 @@
     <numFmt numFmtId="167" formatCode="00000"/>
     <numFmt numFmtId="168" formatCode="[&lt;=9999999]###\-####;###\-###\-####"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="3"/>
@@ -255,15 +256,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF333F4F"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -568,7 +560,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -632,9 +624,6 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="14" xfId="2" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -665,18 +654,15 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="14" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -692,26 +678,23 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="27">
-    <cellStyle name="Bottom Border" xfId="24"/>
-    <cellStyle name="Date" xfId="15"/>
+    <cellStyle name="Bottom Border" xfId="24" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Date" xfId="15" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Ênfase1" xfId="12" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Hiperlink" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" customBuiltin="1"/>
-    <cellStyle name="Invoice description" xfId="21"/>
-    <cellStyle name="Invoice no. &amp; contact info" xfId="22"/>
-    <cellStyle name="Left Align" xfId="13"/>
+    <cellStyle name="Invoice description" xfId="21" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Invoice no. &amp; contact info" xfId="22" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Left Align" xfId="13" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Moeda" xfId="9" builtinId="4" customBuiltin="1"/>
     <cellStyle name="Moeda [0]" xfId="10" builtinId="7" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Phone" xfId="20"/>
+    <cellStyle name="Phone" xfId="20" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
     <cellStyle name="Porcentagem" xfId="11" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Right Align" xfId="14"/>
-    <cellStyle name="Right Indent" xfId="25"/>
+    <cellStyle name="Right Align" xfId="14" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Right Indent" xfId="25" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
     <cellStyle name="Separador de milhares [0]" xfId="8" builtinId="6" customBuiltin="1"/>
     <cellStyle name="Texto Explicativo" xfId="17" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Título" xfId="5" builtinId="15" customBuiltin="1"/>
@@ -719,11 +702,11 @@
     <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="16" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Título 4" xfId="6" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Top align" xfId="23"/>
+    <cellStyle name="Top align" xfId="23" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vírgula" xfId="7" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Zip Code" xfId="19"/>
-    <cellStyle name="znavigation cells" xfId="26"/>
+    <cellStyle name="Zip Code" xfId="19" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="znavigation cells" xfId="26" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
   </cellStyles>
   <dxfs count="14">
     <dxf>
@@ -880,7 +863,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Service Invoice" pivot="0" count="4">
+    <tableStyle name="Service Invoice" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="13"/>
       <tableStyleElement type="headerRow" dxfId="12"/>
       <tableStyleElement type="totalRow" dxfId="11"/>
@@ -915,10 +898,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1">
+        <xdr:cNvPr id="2" name="">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A1FD4469-38C1-4A3D-A0A2-66BEA12DD7B8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1FD4469-38C1-4A3D-A0A2-66BEA12DD7B8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1173,7 +1156,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
@@ -1181,10 +1164,10 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C3" sqref="C3:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
     <col min="2" max="5" width="15" customWidth="1"/>
@@ -1195,8 +1178,8 @@
     <col min="10" max="10" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:11" s="3" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1"/>
+    <row r="2" spans="1:11" s="3" customFormat="1" ht="7.5" customHeight="1">
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -1204,16 +1187,16 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="30" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="36" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="28" t="s">
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="27" t="s">
         <v>1</v>
       </c>
       <c r="H3" s="3"/>
@@ -1223,48 +1206,48 @@
       </c>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="30" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="12"/>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="26"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="B5" s="12"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="40"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="38"/>
       <c r="F5" s="13"/>
-      <c r="G5" s="23"/>
-    </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="24"/>
-      <c r="C6" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="41" t="s">
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="B6" s="23"/>
+      <c r="C6" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="D6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="E6" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="34"/>
-    </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="32"/>
+    </row>
+    <row r="7" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
       <c r="D7" s="18"/>
@@ -1272,58 +1255,58 @@
       <c r="F7" s="19"/>
       <c r="G7" s="20"/>
     </row>
-    <row r="8" spans="1:11" s="3" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="25"/>
+    <row r="8" spans="1:11" s="3" customFormat="1" ht="7.5" customHeight="1">
+      <c r="B8" s="24"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="30" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="15"/>
-      <c r="C9" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="26"/>
+      <c r="C9" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="25"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="30" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="C10" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="D10" s="33" t="s">
         <v>12</v>
       </c>
+      <c r="E10" s="33" t="s">
+        <v>13</v>
+      </c>
       <c r="F10" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="30" customHeight="1">
       <c r="A11" s="3"/>
-      <c r="B11" s="30" t="s">
-        <v>15</v>
+      <c r="B11" s="29" t="s">
+        <v>16</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -1335,10 +1318,10 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
     </row>
-    <row r="12" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="30" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -1350,10 +1333,10 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="30" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -1365,10 +1348,10 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="30" customHeight="1">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -1380,10 +1363,10 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="30" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -1395,10 +1378,10 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
-    <row r="16" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="30" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -1410,10 +1393,10 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
-    <row r="17" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="30" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -1425,10 +1408,10 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
-    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="30" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -1440,10 +1423,10 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
     </row>
-    <row r="19" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="30" customHeight="1">
       <c r="A19" s="3"/>
       <c r="B19" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -1455,10 +1438,10 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="30" customHeight="1">
       <c r="A20" s="3"/>
       <c r="B20" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -1470,7 +1453,7 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="30" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1482,7 +1465,7 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="30" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1494,7 +1477,7 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="30" customHeight="1">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1506,7 +1489,7 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="30" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1518,7 +1501,7 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="30" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1530,7 +1513,7 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
     </row>
-    <row r="26" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="30" customHeight="1">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1542,7 +1525,7 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="30" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1554,7 +1537,7 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
     </row>
-    <row r="28" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="30" customHeight="1">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1566,7 +1549,7 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
     </row>
-    <row r="29" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="30" customHeight="1">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1578,7 +1561,7 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
     </row>
-    <row r="30" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="30" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1590,7 +1573,7 @@
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
     </row>
-    <row r="31" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="30" customHeight="1">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1602,7 +1585,7 @@
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
     </row>
-    <row r="32" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="30" customHeight="1">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1614,7 +1597,7 @@
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
     </row>
-    <row r="33" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="30" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1626,7 +1609,7 @@
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
     </row>
-    <row r="34" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="30" customHeight="1">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1638,7 +1621,7 @@
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
     </row>
-    <row r="35" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="30" customHeight="1">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1650,7 +1633,7 @@
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
     </row>
-    <row r="36" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="30" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1662,7 +1645,7 @@
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
     </row>
-    <row r="37" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="30" customHeight="1">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1674,7 +1657,7 @@
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
     </row>
-    <row r="38" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="30" customHeight="1">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1686,7 +1669,7 @@
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
     </row>
-    <row r="39" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="30" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1698,7 +1681,7 @@
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
     </row>
-    <row r="40" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="30" customHeight="1">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1710,7 +1693,7 @@
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
     </row>
-    <row r="41" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="30" customHeight="1">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1722,7 +1705,7 @@
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
     </row>
-    <row r="42" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="30" customHeight="1">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1734,7 +1717,7 @@
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
     </row>
-    <row r="43" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" ht="30" customHeight="1">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1746,7 +1729,7 @@
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
     </row>
-    <row r="44" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" ht="30" customHeight="1">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1758,7 +1741,7 @@
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
     </row>
-    <row r="45" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" ht="30" customHeight="1">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1770,7 +1753,7 @@
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
     </row>
-    <row r="46" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" ht="30" customHeight="1">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -1782,7 +1765,7 @@
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
     </row>
-    <row r="47" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" ht="30" customHeight="1">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -1794,7 +1777,7 @@
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
     </row>
-    <row r="48" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" ht="30" customHeight="1">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1806,7 +1789,7 @@
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
     </row>
-    <row r="49" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="30" customHeight="1">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -1818,7 +1801,7 @@
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
     </row>
-    <row r="50" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="30" customHeight="1">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -1830,7 +1813,7 @@
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
     </row>
-    <row r="51" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="30" customHeight="1">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -1842,7 +1825,7 @@
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
     </row>
-    <row r="52" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="30" customHeight="1">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -1854,7 +1837,7 @@
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
     </row>
-    <row r="53" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" ht="30" customHeight="1">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -1866,7 +1849,7 @@
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
     </row>
-    <row r="54" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="30" customHeight="1">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -1881,10 +1864,10 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" sort="0"/>
   <mergeCells count="4">
-    <mergeCell ref="D3:E3"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="D5:E5"/>
+    <mergeCell ref="C3:F3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B7:F7 D6:G6">
@@ -1932,25 +1915,25 @@
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
+  <conditionalFormatting sqref="C3">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="872" yWindow="452" count="8">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select customer name from the list. Select CANCEL, then press ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" prompt="Select customer name in this cell. Press ALT+DOWN ARROW to open drop-down list, then ENTER to make selection. Add more customers to Customers worksheet to expand selection list" sqref="B9:B20">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select customer name from the list. Select CANCEL, then press ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" prompt="Select customer name in this cell. Press ALT+DOWN ARROW to open drop-down list, then ENTER to make selection. Add more customers to Customers worksheet to expand selection list" sqref="B9:B20" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>CustomerLookup</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create Service Invoice in this workbook. Enter company &amp; invoice details in this worksheet, &amp; customer details in Customers worksheet. Select cell J1 to navigate to Customers worksheet" sqref="A3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Enter company name in below cell. Enter Invoice Number, Invoice Date and Date Due in cells H1, H2 and H3" sqref="B4:B5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Customer Phone number is automatically updated in cell at right" sqref="C9 C10"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter invoicing company phone number in cell at right" sqref="C4:C5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigation link to Customers worksheet. This cell will not print" sqref="J3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Invoice Date in cell at right" sqref="G4:G7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter invoicing company email address in this cell" sqref="D5 B3 E7:F7 B7:C7 B6:G6 D3 G3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create Service Invoice in this workbook. Enter company &amp; invoice details in this worksheet, &amp; customer details in Customers worksheet. Select cell J1 to navigate to Customers worksheet" sqref="A3" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Enter company name in below cell. Enter Invoice Number, Invoice Date and Date Due in cells H1, H2 and H3" sqref="B4:B5" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Customer Phone number is automatically updated in cell at right" sqref="C9 C10" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter invoicing company phone number in cell at right" sqref="C4:C5" xr:uid="{00000000-0002-0000-0000-00002E000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigation link to Customers worksheet. This cell will not print" sqref="J3" xr:uid="{00000000-0002-0000-0000-000030000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Invoice Date in cell at right" sqref="G4:G7" xr:uid="{00000000-0002-0000-0000-000019000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter invoicing company email address in this cell" sqref="D5 B3 E7:F7 B7:C7 B6:G6 C3 G3" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="J3" location="Customers!A1" tooltip="Select to navigate to Customers worksheet" display="Customers"/>
+    <hyperlink ref="J3" location="Customers!A1" tooltip="Select to navigate to Customers worksheet" display="Customers" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>